<commit_message>
one more test for QUERY is added, util function for Range to Cell is added
</commit_message>
<xml_diff>
--- a/calculation-engine/engine-tests/engine-it/src/test/resources/datamodel/Skills_Sql_Table_Test.xlsx
+++ b/calculation-engine/engine-tests/engine-it/src/test/resources/datamodel/Skills_Sql_Table_Test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5400" windowWidth="24150" windowHeight="11325"/>
+    <workbookView xWindow="0" yWindow="6750" windowWidth="24150" windowHeight="11325"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>Formula</t>
   </si>
@@ -385,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,6 +526,24 @@
         <v>#REF!</v>
       </c>
     </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="e">
+        <f ca="1">INDEX(QUERY("SkillsForLevelOfEnglish","A11",C13:E13),2,1)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>3.8</v>
+      </c>
+      <c r="D13">
+        <v>2.4</v>
+      </c>
+      <c r="E13">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
performance test for QUERY with cache is added
</commit_message>
<xml_diff>
--- a/calculation-engine/engine-tests/engine-it/src/test/resources/datamodel/Skills_Sql_Table_Test.xlsx
+++ b/calculation-engine/engine-tests/engine-it/src/test/resources/datamodel/Skills_Sql_Table_Test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6750" windowWidth="24150" windowHeight="11325"/>
+    <workbookView xWindow="0" yWindow="7200" windowWidth="24150" windowHeight="11325"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>Formula</t>
   </si>
@@ -385,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,6 +544,33 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="e">
+        <f ca="1">QUERY("AllSkills","A14")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="e">
+        <f ca="1">QUERY("AllSkills","A15")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="e">
+        <f ca="1">QUERY("AllSkills","A16")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
performance tests are added #95, #73, #66
</commit_message>
<xml_diff>
--- a/calculation-engine/engine-tests/engine-it/src/test/resources/datamodel/Skills_Sql_Table_Test.xlsx
+++ b/calculation-engine/engine-tests/engine-it/src/test/resources/datamodel/Skills_Sql_Table_Test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7200" windowWidth="24150" windowHeight="11325"/>
+    <workbookView xWindow="0" yWindow="7650" windowWidth="24150" windowHeight="11325"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -388,7 +388,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,7 +461,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="e">
-        <f ca="1">INDEX(QUERY("SkillsForNotLevelOfEnglish",C8, D8),2,1)</f>
+        <f ca="1">INDEX(QUERY(C8, D8,"null"),2,1)</f>
         <v>#NAME?</v>
       </c>
       <c r="B8" t="s">

</xml_diff>